<commit_message>
Finish add visit with insurance test
</commit_message>
<xml_diff>
--- a/Automation/src/com/heal/framework/test/test_data.xlsx
+++ b/Automation/src/com/heal/framework/test/test_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian.rosu/qa-automation/Automation/src/main/java/framework/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian.rosu/qa-automation/Automation/src/com/heal/framework/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="440" windowWidth="38400" windowHeight="19640" tabRatio="991" activeTab="1"/>
+    <workbookView xWindow="38400" yWindow="440" windowWidth="38400" windowHeight="21160" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -55,139 +55,139 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Heal4325</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>+1 201-555-555</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>HasMedicareMedicaid</t>
+  </si>
+  <si>
+    <t>PatientFirstname</t>
+  </si>
+  <si>
+    <t>PatientLastname</t>
+  </si>
+  <si>
+    <t>patientx@heal.com</t>
+  </si>
+  <si>
+    <t>+1 201-555-5555</t>
+  </si>
+  <si>
+    <t>DateOfBirth</t>
+  </si>
+  <si>
+    <t>09/09/1989</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Friend</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>ExpiryMonth</t>
+  </si>
+  <si>
+    <t>ExpiryYear</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>4242424242424242</t>
+  </si>
+  <si>
+    <t>CVC</t>
+  </si>
+  <si>
+    <t>CardType</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>AddressType</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Establishment</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>1 Market St</t>
+  </si>
+  <si>
+    <t>HOME</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>gate code 4235</t>
+  </si>
+  <si>
+    <t>MemberId</t>
+  </si>
+  <si>
+    <t>GroupId</t>
+  </si>
+  <si>
+    <t>COST_ESTIMATES_025</t>
+  </si>
+  <si>
+    <t>BC001</t>
+  </si>
+  <si>
+    <t>Payer</t>
+  </si>
+  <si>
+    <t>Anthem Blue Cross</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
     <t>mihaix16@heal.com</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Heal4325</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>+1 201-555-555</t>
-  </si>
-  <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
-    <t>HasMedicareMedicaid</t>
-  </si>
-  <si>
-    <t>PatientFirstname</t>
-  </si>
-  <si>
-    <t>PatientLastname</t>
-  </si>
-  <si>
-    <t>patientx@heal.com</t>
-  </si>
-  <si>
-    <t>+1 201-555-5555</t>
-  </si>
-  <si>
-    <t>DateOfBirth</t>
-  </si>
-  <si>
-    <t>09/09/1989</t>
-  </si>
-  <si>
-    <t>Relationship</t>
-  </si>
-  <si>
-    <t>Friend</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>ExpiryMonth</t>
-  </si>
-  <si>
-    <t>ExpiryYear</t>
-  </si>
-  <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>4242424242424242</t>
-  </si>
-  <si>
-    <t>CVC</t>
-  </si>
-  <si>
-    <t>CardType</t>
-  </si>
-  <si>
-    <t>Visa</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>AddressType</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Establishment</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Instruction</t>
-  </si>
-  <si>
-    <t>1 Market St</t>
-  </si>
-  <si>
-    <t>HOME</t>
-  </si>
-  <si>
-    <t>San Francisco</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>gate code 4235</t>
-  </si>
-  <si>
-    <t>MemberId</t>
-  </si>
-  <si>
-    <t>GroupId</t>
-  </si>
-  <si>
-    <t>COST_ESTIMATES_025</t>
-  </si>
-  <si>
-    <t>BC001</t>
-  </si>
-  <si>
-    <t>Payer</t>
-  </si>
-  <si>
-    <t>Anthem Blue Cross</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>California</t>
   </si>
 </sst>
 </file>
@@ -257,12 +257,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -649,69 +649,69 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>90210</v>
+        <v>94105</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>123</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -727,15 +727,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>2015555555</v>
@@ -743,10 +743,10 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -784,10 +784,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="b">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
@@ -797,92 +797,92 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>90210</v>
+        <v>94105</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
         <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14">
         <v>2015555555</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>2022</v>
@@ -937,15 +937,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>314</v>
@@ -953,10 +953,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added method for deleting profiles
</commit_message>
<xml_diff>
--- a/Automation/src/com/heal/framework/test/test_data.xlsx
+++ b/Automation/src/com/heal/framework/test/test_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/src/com/heal/framework/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian.rosu/qa-automation/Automation/src/com/heal/framework/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="991"/>
+    <workbookView xWindow="39720" yWindow="1280" windowWidth="38400" windowHeight="19600" tabRatio="991" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Account" sheetId="1" r:id="rId1"/>
@@ -611,7 +611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>